<commit_message>
bug from rounding fixed
</commit_message>
<xml_diff>
--- a/Unity/docs/unityvektor_to_pic_vektor_compare.xlsx
+++ b/Unity/docs/unityvektor_to_pic_vektor_compare.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loahc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loahc\Documents\GitHub\Thesis_HJC885\Unity\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9025E201-AE42-4D92-AE14-15A8FC0A5162}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C6D0AB-6534-4C2A-90BE-5BE51876CA65}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21105" yWindow="3435" windowWidth="15330" windowHeight="6705" xr2:uid="{DFEE8D8A-1C88-422E-A3BD-FDFB0F1D6172}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DFEE8D8A-1C88-422E-A3BD-FDFB0F1D6172}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>alltime</t>
   </si>
@@ -88,12 +88,48 @@
   </si>
   <si>
     <t>(Mennyi le)</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>first pos</t>
+  </si>
+  <si>
+    <t>second pos</t>
+  </si>
+  <si>
+    <t>First pos roboteyes</t>
+  </si>
+  <si>
+    <t>Second pos roboteyes</t>
+  </si>
+  <si>
+    <t>ROBOTEYES</t>
+  </si>
+  <si>
+    <t>BULLETPOSWORLD</t>
+  </si>
+  <si>
+    <t>0,2 sec</t>
+  </si>
+  <si>
+    <t>2 sec</t>
+  </si>
+  <si>
+    <t>x-&gt;y</t>
+  </si>
+  <si>
+    <t>"55/9 0,2-nként"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -127,12 +163,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -447,19 +573,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF25EF4-4D28-4355-B3DA-BB4CF405D23E}">
-  <dimension ref="A1:AC32"/>
+  <dimension ref="A1:AI67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="G24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -1582,8 +1709,1160 @@
         <v>-46</v>
       </c>
     </row>
+    <row r="33" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>25</v>
+      </c>
+      <c r="U33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="9:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M34" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="4"/>
+      <c r="M35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="4"/>
+      <c r="Q35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R35" s="3"/>
+      <c r="S35" s="4"/>
+      <c r="U35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V35" s="3"/>
+      <c r="W35" s="4"/>
+      <c r="Y35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="4"/>
+      <c r="AC35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD35" s="3"/>
+      <c r="AE35" s="4"/>
+    </row>
+    <row r="36" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I36" s="5">
+        <v>5</v>
+      </c>
+      <c r="J36" s="6">
+        <v>0</v>
+      </c>
+      <c r="K36" s="7">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1"/>
+      <c r="M36" s="5">
+        <v>-9</v>
+      </c>
+      <c r="N36" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="O36" s="7">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="5">
+        <v>0</v>
+      </c>
+      <c r="R36" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="S36" s="7">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1"/>
+      <c r="U36" s="5">
+        <f>AC36-Y36</f>
+        <v>0</v>
+      </c>
+      <c r="V36" s="6">
+        <f>AD36-Z36</f>
+        <v>-55</v>
+      </c>
+      <c r="W36" s="7">
+        <f>AE36-AA36</f>
+        <v>0</v>
+      </c>
+      <c r="Y36" s="5">
+        <v>959.5</v>
+      </c>
+      <c r="Z36" s="6">
+        <v>653.5</v>
+      </c>
+      <c r="AA36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="5">
+        <v>959.5</v>
+      </c>
+      <c r="AD36" s="6">
+        <v>598.5</v>
+      </c>
+      <c r="AE36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH36" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI36">
+        <f>V36/(M36-Q36)</f>
+        <v>6.1111111111111107</v>
+      </c>
+    </row>
+    <row r="37" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I37" s="5">
+        <v>4</v>
+      </c>
+      <c r="J37" s="6">
+        <v>0</v>
+      </c>
+      <c r="K37" s="7">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1"/>
+      <c r="M37" s="5">
+        <v>-9.1999999999999993</v>
+      </c>
+      <c r="N37" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="O37" s="7">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="5">
+        <v>-2</v>
+      </c>
+      <c r="R37" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="S37" s="7">
+        <v>0</v>
+      </c>
+      <c r="T37" s="1"/>
+      <c r="U37" s="5">
+        <f>AC37-Y37</f>
+        <v>0</v>
+      </c>
+      <c r="V37" s="6">
+        <f>AD37-Z37</f>
+        <v>-36</v>
+      </c>
+      <c r="W37" s="7">
+        <f>AE37-AA37</f>
+        <v>0</v>
+      </c>
+      <c r="Y37" s="5">
+        <v>959.5</v>
+      </c>
+      <c r="Z37" s="6">
+        <v>633.5</v>
+      </c>
+      <c r="AA37" s="7"/>
+      <c r="AC37" s="5">
+        <v>959.5</v>
+      </c>
+      <c r="AD37" s="6">
+        <v>597.5</v>
+      </c>
+      <c r="AE37" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="7"/>
+      <c r="AI37">
+        <f>V37/(M37-Q37)</f>
+        <v>5.0000000000000009</v>
+      </c>
+    </row>
+    <row r="38" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I38" s="5"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="5">
+        <f t="shared" ref="U38:W64" si="6">AC38-Y38</f>
+        <v>0</v>
+      </c>
+      <c r="V38" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W38" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y38" s="5"/>
+      <c r="Z38" s="6"/>
+      <c r="AA38" s="7"/>
+      <c r="AC38" s="5"/>
+      <c r="AD38" s="6"/>
+      <c r="AE38" s="7"/>
+      <c r="AH38" s="7"/>
+    </row>
+    <row r="39" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I39" s="5"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W39" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="5"/>
+      <c r="Z39" s="6"/>
+      <c r="AA39" s="7"/>
+      <c r="AC39" s="5"/>
+      <c r="AD39" s="6"/>
+      <c r="AE39" s="7"/>
+      <c r="AH39" s="7"/>
+    </row>
+    <row r="40" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I40" s="5"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V40" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W40" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="6"/>
+      <c r="AA40" s="7"/>
+      <c r="AC40" s="5"/>
+      <c r="AD40" s="6"/>
+      <c r="AE40" s="7"/>
+      <c r="AH40" s="7"/>
+    </row>
+    <row r="41" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I41" s="5"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V41" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W41" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="6"/>
+      <c r="AA41" s="7"/>
+      <c r="AC41" s="5"/>
+      <c r="AD41" s="6"/>
+      <c r="AE41" s="7"/>
+      <c r="AH41" s="7"/>
+    </row>
+    <row r="42" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I42" s="5"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V42" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W42" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="6"/>
+      <c r="AA42" s="7"/>
+      <c r="AC42" s="5"/>
+      <c r="AD42" s="6"/>
+      <c r="AE42" s="7"/>
+      <c r="AH42" s="7"/>
+    </row>
+    <row r="43" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I43" s="5"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V43" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W43" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="6"/>
+      <c r="AA43" s="7"/>
+      <c r="AC43" s="5"/>
+      <c r="AD43" s="6"/>
+      <c r="AE43" s="7"/>
+      <c r="AH43" s="7"/>
+    </row>
+    <row r="44" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I44" s="5"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V44" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W44" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="6"/>
+      <c r="AA44" s="7"/>
+      <c r="AC44" s="5"/>
+      <c r="AD44" s="6"/>
+      <c r="AE44" s="7"/>
+      <c r="AH44" s="7"/>
+    </row>
+    <row r="45" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I45" s="5"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V45" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W45" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="6"/>
+      <c r="AA45" s="7"/>
+      <c r="AC45" s="5"/>
+      <c r="AD45" s="6"/>
+      <c r="AE45" s="7"/>
+      <c r="AH45" s="7"/>
+    </row>
+    <row r="46" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I46" s="5"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V46" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W46" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="6"/>
+      <c r="AA46" s="7"/>
+      <c r="AC46" s="5"/>
+      <c r="AD46" s="6"/>
+      <c r="AE46" s="7"/>
+      <c r="AH46" s="7"/>
+    </row>
+    <row r="47" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I47" s="5"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="7"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V47" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W47" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="6"/>
+      <c r="AA47" s="7"/>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="6"/>
+      <c r="AE47" s="7"/>
+      <c r="AH47" s="7"/>
+    </row>
+    <row r="48" spans="9:35" x14ac:dyDescent="0.25">
+      <c r="I48" s="5"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="6"/>
+      <c r="S48" s="7"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V48" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W48" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="6"/>
+      <c r="AA48" s="7"/>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="6"/>
+      <c r="AE48" s="7"/>
+      <c r="AH48" s="7"/>
+    </row>
+    <row r="49" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I49" s="5"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V49" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W49" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="6"/>
+      <c r="AA49" s="7"/>
+      <c r="AC49" s="5"/>
+      <c r="AD49" s="6"/>
+      <c r="AE49" s="7"/>
+      <c r="AH49" s="7"/>
+    </row>
+    <row r="50" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I50" s="5"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V50" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W50" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y50" s="5"/>
+      <c r="Z50" s="6"/>
+      <c r="AA50" s="7"/>
+      <c r="AC50" s="5"/>
+      <c r="AD50" s="6"/>
+      <c r="AE50" s="7"/>
+      <c r="AH50" s="7"/>
+    </row>
+    <row r="51" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I51" s="5"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="6"/>
+      <c r="S51" s="7"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V51" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W51" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="6"/>
+      <c r="AA51" s="7"/>
+      <c r="AC51" s="5"/>
+      <c r="AD51" s="6"/>
+      <c r="AE51" s="7"/>
+      <c r="AH51" s="7"/>
+    </row>
+    <row r="52" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I52" s="5"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="7"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V52" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W52" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y52" s="5"/>
+      <c r="Z52" s="6"/>
+      <c r="AA52" s="7"/>
+      <c r="AC52" s="5"/>
+      <c r="AD52" s="6"/>
+      <c r="AE52" s="7"/>
+      <c r="AH52" s="7"/>
+    </row>
+    <row r="53" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I53" s="5"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="7"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V53" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W53" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="6"/>
+      <c r="AA53" s="7"/>
+      <c r="AC53" s="5"/>
+      <c r="AD53" s="6"/>
+      <c r="AE53" s="7"/>
+      <c r="AH53" s="7"/>
+    </row>
+    <row r="54" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I54" s="5"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="6"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V54" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W54" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="6"/>
+      <c r="AA54" s="7"/>
+      <c r="AC54" s="5"/>
+      <c r="AD54" s="6"/>
+      <c r="AE54" s="7"/>
+      <c r="AH54" s="7"/>
+    </row>
+    <row r="55" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I55" s="5"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V55" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W55" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="6"/>
+      <c r="AA55" s="7"/>
+      <c r="AC55" s="5"/>
+      <c r="AD55" s="6"/>
+      <c r="AE55" s="7"/>
+      <c r="AH55" s="7"/>
+    </row>
+    <row r="56" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I56" s="5"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="6"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="6"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V56" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W56" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="6"/>
+      <c r="AA56" s="7"/>
+      <c r="AC56" s="5"/>
+      <c r="AD56" s="6"/>
+      <c r="AE56" s="7"/>
+      <c r="AH56" s="7"/>
+    </row>
+    <row r="57" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I57" s="5"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="6"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V57" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W57" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y57" s="5"/>
+      <c r="Z57" s="6"/>
+      <c r="AA57" s="7"/>
+      <c r="AC57" s="5"/>
+      <c r="AD57" s="6"/>
+      <c r="AE57" s="7"/>
+      <c r="AH57" s="7"/>
+    </row>
+    <row r="58" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I58" s="5"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="7"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V58" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W58" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="6"/>
+      <c r="AA58" s="7"/>
+      <c r="AC58" s="5"/>
+      <c r="AD58" s="6"/>
+      <c r="AE58" s="7"/>
+      <c r="AH58" s="7"/>
+    </row>
+    <row r="59" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I59" s="5"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V59" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W59" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y59" s="5"/>
+      <c r="Z59" s="6"/>
+      <c r="AA59" s="7"/>
+      <c r="AC59" s="5"/>
+      <c r="AD59" s="6"/>
+      <c r="AE59" s="7"/>
+      <c r="AH59" s="7"/>
+    </row>
+    <row r="60" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I60" s="5"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="6"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="6"/>
+      <c r="S60" s="7"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V60" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W60" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y60" s="5"/>
+      <c r="Z60" s="6"/>
+      <c r="AA60" s="7"/>
+      <c r="AC60" s="5"/>
+      <c r="AD60" s="6"/>
+      <c r="AE60" s="7"/>
+      <c r="AH60" s="7"/>
+    </row>
+    <row r="61" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I61" s="5"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="7"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="7"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V61" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W61" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y61" s="5"/>
+      <c r="Z61" s="6"/>
+      <c r="AA61" s="7"/>
+      <c r="AC61" s="5"/>
+      <c r="AD61" s="6"/>
+      <c r="AE61" s="7"/>
+      <c r="AH61" s="7"/>
+    </row>
+    <row r="62" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I62" s="5"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="6"/>
+      <c r="S62" s="7"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V62" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W62" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y62" s="5"/>
+      <c r="Z62" s="6"/>
+      <c r="AA62" s="7"/>
+      <c r="AC62" s="5"/>
+      <c r="AD62" s="6"/>
+      <c r="AE62" s="7"/>
+      <c r="AH62" s="7"/>
+    </row>
+    <row r="63" spans="9:34" x14ac:dyDescent="0.25">
+      <c r="I63" s="5"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="6"/>
+      <c r="S63" s="7"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V63" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W63" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y63" s="5"/>
+      <c r="Z63" s="6"/>
+      <c r="AA63" s="7"/>
+      <c r="AC63" s="5"/>
+      <c r="AD63" s="6"/>
+      <c r="AE63" s="7"/>
+      <c r="AH63" s="7"/>
+    </row>
+    <row r="64" spans="9:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I64" s="8"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="8"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="10"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="8"/>
+      <c r="R64" s="9"/>
+      <c r="S64" s="10"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V64" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W64" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y64" s="8"/>
+      <c r="Z64" s="9"/>
+      <c r="AA64" s="10"/>
+      <c r="AC64" s="8"/>
+      <c r="AD64" s="9"/>
+      <c r="AE64" s="10"/>
+      <c r="AH64" s="7"/>
+    </row>
+    <row r="65" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+      <c r="Y65" s="1"/>
+      <c r="Z65" s="1"/>
+      <c r="AA65" s="1"/>
+      <c r="AB65" s="1"/>
+      <c r="AC65" s="1"/>
+      <c r="AD65" s="1"/>
+      <c r="AE65" s="1"/>
+    </row>
+    <row r="66" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+      <c r="AD66" s="1"/>
+      <c r="AE66" s="1"/>
+    </row>
+    <row r="67" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+      <c r="AD67" s="1"/>
+      <c r="AE67" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>